<commit_message>
Changed cuda code time measurement. Increased occupancy for rendering
But fps now 2 times lower, but cuda occupancy is 55% instead of 11%
And in time measurements I removed memcpy and cudaMalloc from function and now it approx 100 times faster
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT\Summer_school\Mandelbrot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\MIPT\YandexDisk\PC ANDREY-MIPT\MIPT\Summer_school\Mandelbrot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F20E63F-5403-4503-80A4-D097837ED505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC18CD0-B255-42B0-9069-D1C93C49A573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
   <si>
     <t>Функция</t>
   </si>
   <si>
-    <t>Процессор</t>
-  </si>
-  <si>
     <t>SISD</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>SIMDT_CPU</t>
   </si>
   <si>
-    <t>SIMT_GPU</t>
-  </si>
-  <si>
     <t>Кол-во кадров</t>
   </si>
   <si>
@@ -92,10 +86,22 @@
     <t>epsilon</t>
   </si>
   <si>
-    <t>Intel…</t>
-  </si>
-  <si>
     <t>Better</t>
+  </si>
+  <si>
+    <t>SIMT_GPU (memcpy + malloc)</t>
+  </si>
+  <si>
+    <t>SIMT_GPU (100% CUDA load)</t>
+  </si>
+  <si>
+    <t>Процессор Intel…</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>float</t>
   </si>
 </sst>
 </file>
@@ -129,10 +135,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -142,10 +157,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,83 +445,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="K3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="L3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="Q3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -526,10 +652,37 @@
       <c r="I4">
         <v>10000</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>500</v>
+      </c>
+      <c r="M4">
+        <v>1000</v>
+      </c>
+      <c r="N4">
+        <v>1000</v>
+      </c>
+      <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="P4">
+        <v>500</v>
+      </c>
+      <c r="Q4">
+        <v>10000</v>
+      </c>
+      <c r="R4">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -555,10 +708,16 @@
       <c r="I5">
         <v>107222543980</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="3">
+        <v>25775465464</v>
+      </c>
+      <c r="R5">
+        <v>10060753250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -584,8 +743,14 @@
       <c r="I6">
         <v>107241941790</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="3">
+        <v>25771587240</v>
+      </c>
+      <c r="R6">
+        <v>10436190602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>3</v>
       </c>
@@ -610,8 +775,14 @@
       <c r="I7">
         <v>107342154336</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="3">
+        <v>25881555010</v>
+      </c>
+      <c r="R7">
+        <v>10182601584</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>4</v>
       </c>
@@ -636,8 +807,14 @@
       <c r="I8">
         <v>107357704526</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="3">
+        <v>25756207006</v>
+      </c>
+      <c r="R8">
+        <v>9960928686</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>5</v>
       </c>
@@ -662,8 +839,14 @@
       <c r="I9">
         <v>106417628840</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="3">
+        <v>25826079727</v>
+      </c>
+      <c r="R9">
+        <v>9895324412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>6</v>
       </c>
@@ -688,8 +871,14 @@
       <c r="I10">
         <v>106939689682</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="3">
+        <v>25994572634</v>
+      </c>
+      <c r="R10">
+        <v>10401615658</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>7</v>
       </c>
@@ -714,10 +903,19 @@
       <c r="I11">
         <v>108711687774</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="3">
+        <v>26107940746</v>
+      </c>
+      <c r="R11">
+        <v>10163074115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -750,313 +948,679 @@
         <f t="shared" si="0"/>
         <v>10722254.398</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="4">
+        <f>J5/J$4</f>
+        <v>25775.465464000001</v>
+      </c>
+      <c r="K13" s="1">
+        <f>K5/K$4</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" ref="L13:Q13" si="1">L5/L$4</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="1">
+        <f>R5/R$4</f>
+        <v>10060.75325</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" ref="C14:I19" si="1">C6/C$4</f>
+        <f t="shared" ref="C14:I19" si="2">C6/C$4</f>
         <v>180519238.74000001</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>79736230.986000001</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53269038.245999999</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24244795.658</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>248722111.61000001</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>210089317.31600001</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10724194.179</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="4">
+        <f>J6/J$4</f>
+        <v>25771.587240000001</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" ref="K14:Q14" si="3">K6/K$4</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="1">
+        <f>R6/R$4</f>
+        <v>10436.190602000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>181204500.00999999</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77715590.821999997</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53382899.549999997</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17768688.092999998</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>248286821.22</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>207856845.50400001</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10734215.433599999</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="4">
+        <f>J7/J$4</f>
+        <v>25881.55501</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" ref="K15:Q15" si="4">K7/K$4</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="1">
+        <f>R7/R$4</f>
+        <v>10182.601584</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>4</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>182504206.75999999</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>79940166.187999994</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53499355.030000001</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15308442.219000001</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>251870055.63999999</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>208225704.072</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10735770.4526</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="4">
+        <f>J8/J$4</f>
+        <v>25756.207006000001</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" ref="K16:Q16" si="5">K8/K$4</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="1">
+        <f>R8/R$4</f>
+        <v>9960.9286859999993</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>5</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>181655864.86000001</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>81176496.209999993</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53634405.847999997</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13999847.707</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>248247976.58000001</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>207830261.19600001</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10641762.884</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="4">
+        <f>J9/J$4</f>
+        <v>25826.079727</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" ref="K17:Q17" si="6">K9/K$4</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="1">
+        <f>R9/R$4</f>
+        <v>9895.3244119999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>6</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>181034098.69999999</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80114917.159999996</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53647744.207999997</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13290874.267000001</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>249275386</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>211084821.02399999</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10693968.9682</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="4">
+        <f>J10/J$4</f>
+        <v>25994.572634</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" ref="K18:Q18" si="7">K10/K$4</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="1">
+        <f>R10/R$4</f>
+        <v>10401.615658000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>7</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>181514081.84999999</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>79821410.057999998</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53381160.626000002</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14257144.582</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>248009346.03999999</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>207114519.71599999</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10871168.7774</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J19" s="4">
+        <f>J11/J$4</f>
+        <v>26107.940746</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" ref="K19:Q19" si="8">K11/K$4</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="1">
+        <f>R11/R$4</f>
+        <v>10163.074114999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C21" s="1">
         <f>AVERAGE(C13:C19)</f>
         <v>181157890.66285712</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" ref="D21:I21" si="2">AVERAGE(D13:D19)</f>
+        <f t="shared" ref="D21:I21" si="9">AVERAGE(D13:D19)</f>
         <v>79609068.871999994</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>53578927.636285707</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>16254544.689571429</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>248969413.3385714</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>208962895.48342857</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>10731905.013257144</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="4">
+        <f t="shared" ref="J21:K21" si="10">AVERAGE(J13:J19)</f>
+        <v>25873.343975285716</v>
+      </c>
+      <c r="K21" s="1">
+        <f>AVERAGE(K13:K19)</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" ref="L21:R21" si="11">AVERAGE(L13:L19)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="11"/>
+        <v>10157.212615285714</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C22" s="1">
         <f>_xlfn.STDEV.S(C13:C19)/SQRT(7)</f>
         <v>338658.67073393404</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" ref="D22:I22" si="3">_xlfn.STDEV.S(D13:D19)/SQRT(7)</f>
+        <f t="shared" ref="D22:I22" si="12">_xlfn.STDEV.S(D13:D19)/SQRT(7)</f>
         <v>413810.15823172603</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>121689.19357609896</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>1436686.2537327744</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>507817.89801555627</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>592030.78530242969</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>26336.654697752376</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J22" s="4">
+        <f t="shared" ref="J22:K22" si="13">_xlfn.STDEV.S(J13:J19)/SQRT(7)</f>
+        <v>50.163795638764697</v>
+      </c>
+      <c r="K22" s="1">
+        <f>_xlfn.STDEV.S(K13:K19)/SQRT(7)</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" ref="L22:R22" si="14">_xlfn.STDEV.S(L13:L19)/SQRT(7)</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="1">
+        <f t="shared" si="14"/>
+        <v>77.867063508724897</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C23" s="2">
         <f>C22/C21</f>
         <v>1.869411646905256E-3</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" ref="D23:I23" si="4">D22/D21</f>
+        <f t="shared" ref="D23:I23" si="15">D22/D21</f>
         <v>5.1980278641001769E-3</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>2.2712136831511791E-3</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>8.8386742364707505E-2</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>2.0396798594893221E-3</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>2.833186168926242E-3</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>2.4540521617754398E-3</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J23" s="5">
+        <f t="shared" ref="J23:K23" si="16">J22/J21</f>
+        <v>1.9388215024189097E-3</v>
+      </c>
+      <c r="K23" s="2" t="e">
+        <f>K22/K21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L23" s="2" t="e">
+        <f t="shared" ref="L23:R23" si="17">L22/L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M23" s="2" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N23" s="2" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O23" s="2" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P23" s="2" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q23" s="2" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R23" s="2">
+        <f t="shared" si="17"/>
+        <v>7.6661842631453626E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:F25" si="5">$C$21/C21</f>
+        <f t="shared" ref="C25:F25" si="18">$C$21/C21</f>
         <v>1</v>
       </c>
       <c r="D25">
@@ -1064,11 +1628,11 @@
         <v>2.2755936381335289</v>
       </c>
       <c r="E25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>3.3811406583690196</v>
       </c>
       <c r="F25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>11.145060912046597</v>
       </c>
       <c r="G25">
@@ -1076,15 +1640,55 @@
         <v>1</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25:I25" si="6">$G$21/H21</f>
+        <f t="shared" ref="H25:J25" si="19">$G$21/H21</f>
         <v>1.1914527350063231</v>
       </c>
       <c r="I25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>23.198995241853051</v>
       </c>
+      <c r="J25" s="3">
+        <f>$G$21/J21</f>
+        <v>9622.6221696116136</v>
+      </c>
+      <c r="K25" t="e">
+        <f t="shared" ref="K25:N25" si="20">$C$21/K21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L25" t="e">
+        <f>$C$21/L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M25" t="e">
+        <f t="shared" ref="M25:P25" si="21">$C$21/M21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N25" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O25" t="e">
+        <f>$G$21/O21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P25" t="e">
+        <f t="shared" ref="P25:R25" si="22">$G$21/P21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q25" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R25">
+        <f>$G$21/R21</f>
+        <v>24511.588244583389</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>